<commit_message>
EPBDS-6855 Make test output more descriptive
</commit_message>
<xml_diff>
--- a/Util/openl-maven-plugin/it/openl-tests-failure/src/main/openl/rules/SimpleRules.xlsx
+++ b/Util/openl-maven-plugin/it/openl-tests-failure/src/main/openl/rules/SimpleRules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
   <si>
     <t>Greeting</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>Test Greeting GreetingTest</t>
+  </si>
+  <si>
+    <t>Test Greeting GreetingSuccessful1</t>
+  </si>
+  <si>
+    <t>Test Greeting GreetingSuccessful2</t>
   </si>
 </sst>
 </file>
@@ -601,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G9"/>
+  <dimension ref="B2:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +618,7 @@
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="32.42578125" customWidth="1"/>
     <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
@@ -703,11 +709,112 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="10">
+        <v>25</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F11" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F14" s="10">
+        <v>7</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F15" s="10">
+        <v>13</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F16" s="10">
+        <v>22</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F18" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F20" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="10">
+        <v>7</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F22" s="10">
+        <v>13</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F23" s="10">
+        <v>22</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F18:G18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>